<commit_message>
Update for new fish tagged and receiver download 4
</commit_message>
<xml_diff>
--- a/shapefiles/deployments_notes.xlsx
+++ b/shapefiles/deployments_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fwcc-my.sharepoint.com/personal/jonathan_peake_myfwc_com/Documents/Documents/FIM Data Projects/Robinson Preserve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fwcc-my.sharepoint.com/personal/jonathan_peake_myfwc_com/Documents/Documents/FIM Data Projects/Robinson Preserve/Github/shapefiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C784992-979B-4391-9BCD-42668834C886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{6C784992-979B-4391-9BCD-42668834C886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3977713-0412-4B1D-A8E9-01F17CF5AADC}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" xr2:uid="{D0089CB3-D5AE-4054-B1D9-E5E785F2CA82}"/>
+    <workbookView xWindow="5748" yWindow="1008" windowWidth="23040" windowHeight="12216" xr2:uid="{D0089CB3-D5AE-4054-B1D9-E5E785F2CA82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -203,6 +203,12 @@
   </si>
   <si>
     <t>Longitude_dd</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
   </si>
 </sst>
 </file>
@@ -555,38 +561,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7818636-F325-4D6B-9AF4-530AE89DCB5F}">
-  <dimension ref="A1:V14"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="93.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="93.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -654,7 +660,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44669</v>
       </c>
@@ -722,7 +728,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44669</v>
       </c>
@@ -790,7 +796,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44669</v>
       </c>
@@ -858,7 +864,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44669</v>
       </c>
@@ -926,7 +932,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44669</v>
       </c>
@@ -994,7 +1000,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44669</v>
       </c>
@@ -1062,7 +1068,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44669</v>
       </c>
@@ -1130,7 +1136,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44669</v>
       </c>
@@ -1198,7 +1204,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44669</v>
       </c>
@@ -1266,7 +1272,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44669</v>
       </c>
@@ -1334,7 +1340,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>44669</v>
       </c>
@@ -1402,7 +1408,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>44669</v>
       </c>
@@ -1470,7 +1476,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>44669</v>
       </c>
@@ -1536,6 +1542,41 @@
       </c>
       <c r="V14" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>44986</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15">
+        <v>138847</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15">
+        <v>27</v>
+      </c>
+      <c r="G15">
+        <v>31.254000000000001</v>
+      </c>
+      <c r="H15">
+        <v>27.520900000000001</v>
+      </c>
+      <c r="I15">
+        <v>82</v>
+      </c>
+      <c r="J15">
+        <v>40.381999999999998</v>
+      </c>
+      <c r="K15">
+        <v>82.6730333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix data map issue
</commit_message>
<xml_diff>
--- a/shapefiles/deployments_notes.xlsx
+++ b/shapefiles/deployments_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fwcc-my.sharepoint.com/personal/jonathan_peake_myfwc_com/Documents/Documents/FIM Data Projects/Robinson Preserve/Github/shapefiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{6C784992-979B-4391-9BCD-42668834C886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3977713-0412-4B1D-A8E9-01F17CF5AADC}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{6C784992-979B-4391-9BCD-42668834C886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95801E8D-8FF0-47D3-8BD1-24AD681FC3E7}"/>
   <bookViews>
-    <workbookView xWindow="5748" yWindow="1008" windowWidth="23040" windowHeight="12216" xr2:uid="{D0089CB3-D5AE-4054-B1D9-E5E785F2CA82}"/>
+    <workbookView xWindow="38280" yWindow="2325" windowWidth="29040" windowHeight="15840" xr2:uid="{D0089CB3-D5AE-4054-B1D9-E5E785F2CA82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -209,6 +209,18 @@
   </si>
   <si>
     <t>MS</t>
+  </si>
+  <si>
+    <t>Mead Point #4</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Inactive</t>
   </si>
 </sst>
 </file>
@@ -561,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7818636-F325-4D6B-9AF4-530AE89DCB5F}">
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,20 +591,21 @@
     <col min="8" max="9" width="12.109375" customWidth="1"/>
     <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="93.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="93.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -627,40 +640,43 @@
         <v>55</v>
       </c>
       <c r="L1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>20</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>7</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>8</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>9</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>10</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>11</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44669</v>
       </c>
@@ -671,64 +687,69 @@
         <v>15</v>
       </c>
       <c r="D2">
-        <v>138109</v>
+        <v>138105</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F2">
         <v>27</v>
       </c>
       <c r="G2">
-        <v>29.922000000000001</v>
+        <v>30.908000000000001</v>
       </c>
       <c r="H2">
-        <v>27.498699999999999</v>
+        <f>F2+G2/60</f>
+        <v>27.515133333333335</v>
       </c>
       <c r="I2">
         <v>82</v>
       </c>
       <c r="J2">
-        <v>39.624000000000002</v>
+        <v>41.088999999999999</v>
       </c>
       <c r="K2">
-        <v>82.660399999999996</v>
-      </c>
-      <c r="L2">
-        <v>900</v>
+        <f>I2+J2/60</f>
+        <v>82.684816666666663</v>
+      </c>
+      <c r="L2" t="s">
+        <v>61</v>
       </c>
       <c r="M2">
+        <v>1047</v>
+      </c>
+      <c r="N2">
         <v>1</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>0.25</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>21</v>
       </c>
-      <c r="P2">
-        <v>35.56</v>
-      </c>
       <c r="Q2">
-        <v>55.195</v>
+        <v>34.770000000000003</v>
       </c>
       <c r="R2">
-        <v>53.853000000000002</v>
+        <v>53.978999999999999</v>
       </c>
       <c r="S2">
-        <v>26.3</v>
-      </c>
-      <c r="T2" t="s">
+        <v>52.792000000000002</v>
+      </c>
+      <c r="T2">
+        <v>26.2</v>
+      </c>
+      <c r="U2" t="s">
         <v>17</v>
       </c>
-      <c r="U2">
-        <v>21309027</v>
-      </c>
-      <c r="V2" t="s">
-        <v>19</v>
+      <c r="V2">
+        <v>21309029</v>
+      </c>
+      <c r="W2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44669</v>
       </c>
@@ -739,64 +760,69 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>138101</v>
+        <v>138107</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F3">
         <v>27</v>
       </c>
       <c r="G3">
-        <v>29.594000000000001</v>
+        <v>31.312999999999999</v>
       </c>
       <c r="H3">
-        <v>27.493233333333333</v>
+        <f t="shared" ref="H3:H15" si="0">F3+G3/60</f>
+        <v>27.521883333333335</v>
       </c>
       <c r="I3">
         <v>82</v>
       </c>
       <c r="J3">
-        <v>40.100999999999999</v>
+        <v>40.381999999999998</v>
       </c>
       <c r="K3">
-        <v>82.668350000000004</v>
-      </c>
-      <c r="L3">
-        <v>930</v>
+        <f t="shared" ref="K3:K15" si="1">I3+J3/60</f>
+        <v>82.673033333333336</v>
+      </c>
+      <c r="L3" t="s">
+        <v>59</v>
       </c>
       <c r="M3">
-        <v>1.6</v>
+        <v>1100</v>
       </c>
       <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3">
-        <v>36.369999999999997</v>
+        <v>1.3</v>
+      </c>
+      <c r="O3">
+        <v>0.25</v>
+      </c>
+      <c r="P3" t="s">
+        <v>21</v>
       </c>
       <c r="Q3">
-        <v>56.424999999999997</v>
+        <v>34.21</v>
       </c>
       <c r="R3">
-        <v>54.92</v>
+        <v>53.398000000000003</v>
       </c>
       <c r="S3">
-        <v>26.4</v>
-      </c>
-      <c r="T3" t="s">
+        <v>52.046999999999997</v>
+      </c>
+      <c r="T3">
+        <v>26.1</v>
+      </c>
+      <c r="U3" t="s">
         <v>17</v>
       </c>
-      <c r="U3">
-        <v>21309023</v>
-      </c>
-      <c r="V3" t="s">
-        <v>24</v>
+      <c r="V3">
+        <v>21309024</v>
+      </c>
+      <c r="W3" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44669</v>
       </c>
@@ -807,132 +833,109 @@
         <v>15</v>
       </c>
       <c r="D4">
-        <v>138104</v>
+        <v>138100</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F4">
         <v>27</v>
       </c>
       <c r="G4">
-        <v>30.431000000000001</v>
+        <v>31.413</v>
       </c>
       <c r="H4">
-        <v>27.507183333333334</v>
+        <f t="shared" si="0"/>
+        <v>27.52355</v>
       </c>
       <c r="I4">
         <v>82</v>
       </c>
       <c r="J4">
-        <v>40.508000000000003</v>
+        <v>39.997999999999998</v>
       </c>
       <c r="K4">
-        <v>82.675133333333335</v>
-      </c>
-      <c r="L4">
-        <v>1015</v>
+        <f t="shared" si="1"/>
+        <v>82.666633333333337</v>
+      </c>
+      <c r="L4" t="s">
+        <v>61</v>
       </c>
       <c r="M4">
-        <v>0.8</v>
+        <v>1129</v>
       </c>
       <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
         <v>0.25</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>21</v>
       </c>
-      <c r="P4">
-        <v>36.56</v>
-      </c>
       <c r="Q4">
-        <v>57.18</v>
+        <v>34.22</v>
       </c>
       <c r="R4">
-        <v>55.228000000000002</v>
+        <v>53.470999999999997</v>
       </c>
       <c r="S4">
-        <v>26.8</v>
-      </c>
-      <c r="T4" t="s">
+        <v>52.064</v>
+      </c>
+      <c r="T4">
+        <v>26.4</v>
+      </c>
+      <c r="U4" t="s">
         <v>17</v>
       </c>
-      <c r="U4">
-        <v>21309025</v>
-      </c>
-      <c r="V4" t="s">
-        <v>26</v>
+      <c r="V4">
+        <v>21309026</v>
+      </c>
+      <c r="W4" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>44669</v>
+        <v>44986</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="D5">
-        <v>138105</v>
+        <v>138847</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="F5">
         <v>27</v>
       </c>
       <c r="G5">
-        <v>30.908000000000001</v>
+        <v>31.254000000000001</v>
       </c>
       <c r="H5">
-        <v>27.515133333333335</v>
+        <f t="shared" si="0"/>
+        <v>27.520900000000001</v>
       </c>
       <c r="I5">
         <v>82</v>
       </c>
       <c r="J5">
-        <v>41.088999999999999</v>
+        <v>40.003999999999998</v>
       </c>
       <c r="K5">
-        <v>82.684816666666663</v>
-      </c>
-      <c r="L5">
-        <v>1047</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>0.25</v>
-      </c>
-      <c r="O5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P5">
-        <v>34.770000000000003</v>
-      </c>
-      <c r="Q5">
-        <v>53.978999999999999</v>
-      </c>
-      <c r="R5">
-        <v>52.792000000000002</v>
-      </c>
-      <c r="S5">
-        <v>26.2</v>
-      </c>
-      <c r="T5" t="s">
-        <v>17</v>
-      </c>
-      <c r="U5">
-        <v>21309029</v>
-      </c>
-      <c r="V5" t="s">
-        <v>28</v>
+        <f t="shared" si="1"/>
+        <v>82.66673333333334</v>
+      </c>
+      <c r="L5" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44669</v>
       </c>
@@ -943,64 +946,69 @@
         <v>15</v>
       </c>
       <c r="D6">
-        <v>138107</v>
+        <v>138101</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F6">
         <v>27</v>
       </c>
       <c r="G6">
-        <v>31.327000000000002</v>
+        <v>29.594000000000001</v>
       </c>
       <c r="H6">
-        <v>27.522116666666665</v>
+        <f t="shared" si="0"/>
+        <v>27.493233333333333</v>
       </c>
       <c r="I6">
         <v>82</v>
       </c>
       <c r="J6">
-        <v>40.289000000000001</v>
+        <v>40.100999999999999</v>
       </c>
       <c r="K6">
-        <v>82.671483333333327</v>
-      </c>
-      <c r="L6">
-        <v>1100</v>
+        <f t="shared" si="1"/>
+        <v>82.668350000000004</v>
+      </c>
+      <c r="L6" t="s">
+        <v>59</v>
       </c>
       <c r="M6">
-        <v>1.3</v>
+        <v>930</v>
       </c>
       <c r="N6">
-        <v>0.25</v>
-      </c>
-      <c r="O6" t="s">
-        <v>21</v>
-      </c>
-      <c r="P6">
-        <v>34.21</v>
+        <v>1.6</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
+        <v>23</v>
       </c>
       <c r="Q6">
-        <v>53.398000000000003</v>
+        <v>36.369999999999997</v>
       </c>
       <c r="R6">
-        <v>52.046999999999997</v>
+        <v>56.424999999999997</v>
       </c>
       <c r="S6">
-        <v>26.1</v>
-      </c>
-      <c r="T6" t="s">
+        <v>54.92</v>
+      </c>
+      <c r="T6">
+        <v>26.4</v>
+      </c>
+      <c r="U6" t="s">
         <v>17</v>
       </c>
-      <c r="U6">
-        <v>21309024</v>
-      </c>
-      <c r="V6" t="s">
-        <v>30</v>
+      <c r="V6">
+        <v>21309023</v>
+      </c>
+      <c r="W6" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44669</v>
       </c>
@@ -1011,64 +1019,69 @@
         <v>15</v>
       </c>
       <c r="D7">
-        <v>138100</v>
+        <v>138109</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F7">
         <v>27</v>
       </c>
       <c r="G7">
-        <v>31.413</v>
+        <v>29.922000000000001</v>
       </c>
       <c r="H7">
-        <v>27.52355</v>
+        <f t="shared" si="0"/>
+        <v>27.498699999999999</v>
       </c>
       <c r="I7">
         <v>82</v>
       </c>
       <c r="J7">
-        <v>39.997999999999998</v>
+        <v>39.624000000000002</v>
       </c>
       <c r="K7">
-        <v>82.666633333333337</v>
-      </c>
-      <c r="L7">
-        <v>1129</v>
+        <f t="shared" si="1"/>
+        <v>82.660399999999996</v>
+      </c>
+      <c r="L7" t="s">
+        <v>59</v>
       </c>
       <c r="M7">
+        <v>900</v>
+      </c>
+      <c r="N7">
         <v>1</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>0.25</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>21</v>
       </c>
-      <c r="P7">
-        <v>34.22</v>
-      </c>
       <c r="Q7">
-        <v>53.470999999999997</v>
+        <v>35.56</v>
       </c>
       <c r="R7">
-        <v>52.064</v>
+        <v>55.195</v>
       </c>
       <c r="S7">
-        <v>26.4</v>
-      </c>
-      <c r="T7" t="s">
+        <v>53.853000000000002</v>
+      </c>
+      <c r="T7">
+        <v>26.3</v>
+      </c>
+      <c r="U7" t="s">
         <v>17</v>
       </c>
-      <c r="U7">
-        <v>21309026</v>
-      </c>
-      <c r="V7" t="s">
-        <v>32</v>
+      <c r="V7">
+        <v>21309027</v>
+      </c>
+      <c r="W7" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44669</v>
       </c>
@@ -1079,64 +1092,69 @@
         <v>15</v>
       </c>
       <c r="D8">
-        <v>138108</v>
+        <v>138104</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F8">
         <v>27</v>
       </c>
       <c r="G8">
-        <v>31.207000000000001</v>
+        <v>30.431000000000001</v>
       </c>
       <c r="H8">
-        <v>27.520116666666667</v>
+        <f t="shared" si="0"/>
+        <v>27.507183333333334</v>
       </c>
       <c r="I8">
         <v>82</v>
       </c>
       <c r="J8">
-        <v>39.888800000000003</v>
+        <v>40.508000000000003</v>
       </c>
       <c r="K8">
-        <v>82.664813333333328</v>
-      </c>
-      <c r="L8">
-        <v>1308</v>
+        <f t="shared" si="1"/>
+        <v>82.675133333333335</v>
+      </c>
+      <c r="L8" t="s">
+        <v>59</v>
       </c>
       <c r="M8">
-        <v>1.1000000000000001</v>
+        <v>1015</v>
       </c>
       <c r="N8">
-        <v>0.2</v>
-      </c>
-      <c r="O8" t="s">
-        <v>34</v>
+        <v>0.8</v>
+      </c>
+      <c r="O8">
+        <v>0.25</v>
       </c>
       <c r="P8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>23</v>
-      </c>
-      <c r="R8" t="s">
-        <v>23</v>
-      </c>
-      <c r="S8" t="s">
-        <v>23</v>
-      </c>
-      <c r="T8" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="Q8">
+        <v>36.56</v>
+      </c>
+      <c r="R8">
+        <v>57.18</v>
+      </c>
+      <c r="S8">
+        <v>55.228000000000002</v>
+      </c>
+      <c r="T8">
+        <v>26.8</v>
       </c>
       <c r="U8" t="s">
-        <v>23</v>
-      </c>
-      <c r="V8" t="s">
-        <v>35</v>
+        <v>17</v>
+      </c>
+      <c r="V8">
+        <v>21309025</v>
+      </c>
+      <c r="W8" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44669</v>
       </c>
@@ -1147,43 +1165,45 @@
         <v>15</v>
       </c>
       <c r="D9">
-        <v>138103</v>
+        <v>138102</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F9">
         <v>27</v>
       </c>
       <c r="G9">
-        <v>30.726199999999999</v>
+        <v>30.53</v>
       </c>
       <c r="H9">
-        <v>27.512103333333332</v>
+        <f t="shared" si="0"/>
+        <v>27.508833333333332</v>
       </c>
       <c r="I9">
         <v>82</v>
       </c>
       <c r="J9">
-        <v>40.296199999999999</v>
+        <v>40.142000000000003</v>
       </c>
       <c r="K9">
-        <v>82.671603333333337</v>
-      </c>
-      <c r="L9">
-        <v>1324</v>
+        <f t="shared" si="1"/>
+        <v>82.669033333333331</v>
+      </c>
+      <c r="L9" t="s">
+        <v>59</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>1401</v>
       </c>
       <c r="N9">
+        <v>0.9</v>
+      </c>
+      <c r="O9">
         <v>0.1</v>
       </c>
-      <c r="O9" t="s">
-        <v>23</v>
-      </c>
       <c r="P9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q9" t="s">
         <v>23</v>
@@ -1201,10 +1221,13 @@
         <v>23</v>
       </c>
       <c r="V9" t="s">
-        <v>46</v>
+        <v>23</v>
+      </c>
+      <c r="W9" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44669</v>
       </c>
@@ -1215,44 +1238,46 @@
         <v>15</v>
       </c>
       <c r="D10">
-        <v>138109</v>
+        <v>138097</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F10">
         <v>27</v>
       </c>
       <c r="G10">
-        <v>30.734000000000002</v>
+        <v>30.380800000000001</v>
       </c>
       <c r="H10">
-        <v>27.512233333333334</v>
+        <f t="shared" si="0"/>
+        <v>27.506346666666666</v>
       </c>
       <c r="I10">
         <v>82</v>
       </c>
       <c r="J10">
-        <v>40.066000000000003</v>
+        <v>39.981000000000002</v>
       </c>
       <c r="K10">
-        <v>82.667766666666665</v>
-      </c>
-      <c r="L10">
-        <v>1348</v>
+        <f t="shared" si="1"/>
+        <v>82.666349999999994</v>
+      </c>
+      <c r="L10" t="s">
+        <v>59</v>
       </c>
       <c r="M10">
+        <v>1442</v>
+      </c>
+      <c r="N10">
         <v>1.2</v>
       </c>
-      <c r="N10">
-        <v>0.3</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="O10">
+        <v>0.2</v>
+      </c>
+      <c r="P10" t="s">
         <v>42</v>
       </c>
-      <c r="P10" t="s">
-        <v>23</v>
-      </c>
       <c r="Q10" t="s">
         <v>23</v>
       </c>
@@ -1269,10 +1294,13 @@
         <v>23</v>
       </c>
       <c r="V10" t="s">
-        <v>45</v>
+        <v>23</v>
+      </c>
+      <c r="W10" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44669</v>
       </c>
@@ -1283,43 +1311,45 @@
         <v>15</v>
       </c>
       <c r="D11">
-        <v>138102</v>
+        <v>138098</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F11">
         <v>27</v>
       </c>
       <c r="G11">
-        <v>30.53</v>
+        <v>30.516500000000001</v>
       </c>
       <c r="H11">
-        <v>27.508833333333332</v>
+        <f t="shared" si="0"/>
+        <v>27.508608333333335</v>
       </c>
       <c r="I11">
         <v>82</v>
       </c>
       <c r="J11">
-        <v>40.142000000000003</v>
+        <v>40.202800000000003</v>
       </c>
       <c r="K11">
-        <v>82.669033333333331</v>
-      </c>
-      <c r="L11">
-        <v>1401</v>
+        <f t="shared" si="1"/>
+        <v>82.670046666666664</v>
+      </c>
+      <c r="L11" t="s">
+        <v>59</v>
       </c>
       <c r="M11">
+        <v>1408</v>
+      </c>
+      <c r="N11">
         <v>0.9</v>
       </c>
-      <c r="N11">
-        <v>0.1</v>
-      </c>
-      <c r="O11" t="s">
-        <v>21</v>
+      <c r="O11">
+        <v>0.3</v>
       </c>
       <c r="P11" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="Q11" t="s">
         <v>23</v>
@@ -1337,10 +1367,13 @@
         <v>23</v>
       </c>
       <c r="V11" t="s">
-        <v>44</v>
+        <v>23</v>
+      </c>
+      <c r="W11" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>44669</v>
       </c>
@@ -1351,43 +1384,45 @@
         <v>15</v>
       </c>
       <c r="D12">
-        <v>138098</v>
+        <v>138106</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F12">
         <v>27</v>
       </c>
       <c r="G12">
-        <v>30.516500000000001</v>
+        <v>30.734000000000002</v>
       </c>
       <c r="H12">
-        <v>27.508608333333335</v>
+        <f t="shared" si="0"/>
+        <v>27.512233333333334</v>
       </c>
       <c r="I12">
         <v>82</v>
       </c>
       <c r="J12">
-        <v>40.202800000000003</v>
+        <v>40.066000000000003</v>
       </c>
       <c r="K12">
-        <v>82.670046666666664</v>
-      </c>
-      <c r="L12">
-        <v>1408</v>
+        <f t="shared" si="1"/>
+        <v>82.667766666666665</v>
+      </c>
+      <c r="L12" t="s">
+        <v>59</v>
       </c>
       <c r="M12">
-        <v>0.9</v>
+        <v>1348</v>
       </c>
       <c r="N12">
+        <v>1.2</v>
+      </c>
+      <c r="O12">
         <v>0.3</v>
       </c>
-      <c r="O12" t="s">
-        <v>48</v>
-      </c>
       <c r="P12" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="Q12" t="s">
         <v>23</v>
@@ -1405,10 +1440,13 @@
         <v>23</v>
       </c>
       <c r="V12" t="s">
-        <v>50</v>
+        <v>23</v>
+      </c>
+      <c r="W12" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>44669</v>
       </c>
@@ -1419,40 +1457,42 @@
         <v>15</v>
       </c>
       <c r="D13">
-        <v>138009</v>
+        <v>138103</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F13">
         <v>27</v>
       </c>
       <c r="G13">
-        <v>30.390999999999998</v>
+        <v>30.726199999999999</v>
       </c>
       <c r="H13">
-        <v>27.506516666666666</v>
+        <f t="shared" si="0"/>
+        <v>27.512103333333332</v>
       </c>
       <c r="I13">
         <v>82</v>
       </c>
       <c r="J13">
-        <v>40.146000000000001</v>
+        <v>40.296199999999999</v>
       </c>
       <c r="K13">
-        <v>82.6691</v>
-      </c>
-      <c r="L13">
-        <v>1427</v>
+        <f t="shared" si="1"/>
+        <v>82.671603333333337</v>
+      </c>
+      <c r="L13" t="s">
+        <v>59</v>
       </c>
       <c r="M13">
-        <v>1.3</v>
+        <v>1324</v>
       </c>
       <c r="N13">
-        <v>0.2</v>
-      </c>
-      <c r="O13" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>0.1</v>
       </c>
       <c r="P13" t="s">
         <v>23</v>
@@ -1473,10 +1513,13 @@
         <v>23</v>
       </c>
       <c r="V13" t="s">
-        <v>51</v>
+        <v>23</v>
+      </c>
+      <c r="W13" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>44669</v>
       </c>
@@ -1487,43 +1530,45 @@
         <v>15</v>
       </c>
       <c r="D14">
-        <v>138097</v>
+        <v>138108</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="F14">
         <v>27</v>
       </c>
       <c r="G14">
-        <v>30.380800000000001</v>
+        <v>31.207000000000001</v>
       </c>
       <c r="H14">
-        <v>27.506346666666666</v>
+        <f t="shared" si="0"/>
+        <v>27.520116666666667</v>
       </c>
       <c r="I14">
         <v>82</v>
       </c>
       <c r="J14">
-        <v>39.979799999999997</v>
+        <v>39.888800000000003</v>
       </c>
       <c r="K14">
-        <v>82.666330000000002</v>
-      </c>
-      <c r="L14">
-        <v>1442</v>
+        <f t="shared" si="1"/>
+        <v>82.664813333333328</v>
+      </c>
+      <c r="L14" t="s">
+        <v>59</v>
       </c>
       <c r="M14">
-        <v>1.2</v>
+        <v>1308</v>
       </c>
       <c r="N14">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O14">
         <v>0.2</v>
       </c>
-      <c r="O14" t="s">
-        <v>42</v>
-      </c>
       <c r="P14" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="Q14" t="s">
         <v>23</v>
@@ -1541,45 +1586,89 @@
         <v>23</v>
       </c>
       <c r="V14" t="s">
-        <v>53</v>
+        <v>23</v>
+      </c>
+      <c r="W14" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>44986</v>
+        <v>44669</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="D15">
-        <v>138847</v>
+        <v>138099</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="F15">
         <v>27</v>
       </c>
       <c r="G15">
-        <v>31.254000000000001</v>
+        <v>30.390999999999998</v>
       </c>
       <c r="H15">
-        <v>27.520900000000001</v>
+        <f t="shared" si="0"/>
+        <v>27.506516666666666</v>
       </c>
       <c r="I15">
         <v>82</v>
       </c>
       <c r="J15">
-        <v>40.381999999999998</v>
+        <v>40.146000000000001</v>
       </c>
       <c r="K15">
-        <v>82.6730333</v>
+        <f t="shared" si="1"/>
+        <v>82.6691</v>
+      </c>
+      <c r="L15" t="s">
+        <v>59</v>
+      </c>
+      <c r="M15">
+        <v>1427</v>
+      </c>
+      <c r="N15">
+        <v>1.3</v>
+      </c>
+      <c r="O15">
+        <v>0.2</v>
+      </c>
+      <c r="P15" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>23</v>
+      </c>
+      <c r="R15" t="s">
+        <v>23</v>
+      </c>
+      <c r="S15" t="s">
+        <v>23</v>
+      </c>
+      <c r="T15" t="s">
+        <v>23</v>
+      </c>
+      <c r="U15" t="s">
+        <v>23</v>
+      </c>
+      <c r="V15" t="s">
+        <v>23</v>
+      </c>
+      <c r="W15" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W15">
+    <sortCondition ref="E1:E15"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>